<commit_message>
COMPAS data with predictions
</commit_message>
<xml_diff>
--- a/src/random/table_with_COMPAS_attributes.xlsx
+++ b/src/random/table_with_COMPAS_attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caroline\Documents\DTU\Master_thesis\Fairness-oriented-interpretability-of-predictive-algorithms\src\random\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709ACB12-A8F7-4142-B1AB-45D0C16A194B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903E4B20-DDC8-4072-AA53-066F4B12777B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{97F21BEF-DC4A-4CF3-BADD-287AF59747F4}"/>
+    <workbookView xWindow="-105" yWindow="-18120" windowWidth="29040" windowHeight="17640" xr2:uid="{97F21BEF-DC4A-4CF3-BADD-287AF59747F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -716,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB49812-28E9-4CDA-8A32-BA1CE4BF362E}">
   <dimension ref="A1:AN54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -863,7 +863,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:40" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:40" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>48</v>
       </c>

</xml_diff>